<commit_message>
Refactor stamp image loading in DbSeeder for improved path handling
- Enhanced the LoadStampImageBytes method to better resolve image paths, ensuring more reliable loading of stamp images during seeding.
- Updated the project file to include all necessary files from the Data\STAMP directory, improving resource availability for the application.
</commit_message>
<xml_diff>
--- a/CNCToolingDatabase/bin/Debug/net8.0/Data/MASTER - USER.xlsx
+++ b/CNCToolingDatabase/bin/Debug/net8.0/Data/MASTER - USER.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Public\Documents\Tool-Master-Control\Tool-Master-Control\CNCToolingDatabase\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{030FEE93-8B91-470F-A6B2-B5357DA84D05}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13D76624-5036-44F0-A9EC-9B4FE7A49476}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1455" yWindow="3570" windowWidth="21600" windowHeight="11295" xr2:uid="{8271D9D6-2065-419F-AC52-7850B71D4074}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{8271D9D6-2065-419F-AC52-7850B71D4074}"/>
   </bookViews>
   <sheets>
     <sheet name="User" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="31">
   <si>
     <t>No.</t>
   </si>
@@ -118,6 +118,15 @@
   </si>
   <si>
     <t>abc123</t>
+  </si>
+  <si>
+    <t>Stamp Image</t>
+  </si>
+  <si>
+    <t>\STAMP\adib.jamil.PNG</t>
+  </si>
+  <si>
+    <t>\STAMP\hakim.hisham.PNG</t>
   </si>
 </sst>
 </file>
@@ -185,7 +194,10 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="7">
+  <dxfs count="8">
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <numFmt numFmtId="30" formatCode="@"/>
       <fill>
@@ -282,17 +294,18 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{1F9D2975-A917-404F-9FF3-664FDE891014}" name="Table1" displayName="Table1" ref="A1:E11" totalsRowShown="0" headerRowDxfId="6" dataDxfId="5">
-  <autoFilter ref="A1:E11" xr:uid="{1F9D2975-A917-404F-9FF3-664FDE891014}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E10">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{1F9D2975-A917-404F-9FF3-664FDE891014}" name="Table1" displayName="Table1" ref="A1:F11" totalsRowShown="0" headerRowDxfId="7" dataDxfId="6">
+  <autoFilter ref="A1:F11" xr:uid="{1F9D2975-A917-404F-9FF3-664FDE891014}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F10">
     <sortCondition ref="A1:A10"/>
   </sortState>
-  <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{4A87BED8-B1B5-45DE-BB4C-8C3E6116591E}" name="No." dataDxfId="4"/>
-    <tableColumn id="6" xr3:uid="{5E55A1C0-5160-4819-9AC4-BFE97197F01A}" name="Username" dataDxfId="3"/>
-    <tableColumn id="4" xr3:uid="{9E99972C-6257-4496-92A9-7B0B9EFC93FF}" name="Password" dataDxfId="2"/>
-    <tableColumn id="2" xr3:uid="{E05168FF-5C3E-4D5A-B93D-D4D10BF8E5D9}" name="Display Name" dataDxfId="1"/>
-    <tableColumn id="3" xr3:uid="{F3A2A34E-F6A4-4E74-965D-DE476ADF2610}" name="Status" dataDxfId="0"/>
+  <tableColumns count="6">
+    <tableColumn id="1" xr3:uid="{4A87BED8-B1B5-45DE-BB4C-8C3E6116591E}" name="No." dataDxfId="5"/>
+    <tableColumn id="6" xr3:uid="{5E55A1C0-5160-4819-9AC4-BFE97197F01A}" name="Username" dataDxfId="4"/>
+    <tableColumn id="4" xr3:uid="{9E99972C-6257-4496-92A9-7B0B9EFC93FF}" name="Password" dataDxfId="3"/>
+    <tableColumn id="2" xr3:uid="{E05168FF-5C3E-4D5A-B93D-D4D10BF8E5D9}" name="Display Name" dataDxfId="2"/>
+    <tableColumn id="5" xr3:uid="{E0E5F64A-7280-41EB-A7D5-B9BF82770011}" name="Stamp Image" dataDxfId="0"/>
+    <tableColumn id="3" xr3:uid="{F3A2A34E-F6A4-4E74-965D-DE476ADF2610}" name="Status" dataDxfId="1"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -595,10 +608,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2A8EBE31-42AA-4644-A64F-E2B9900B290E}">
-  <dimension ref="A1:E11"/>
+  <dimension ref="A1:F11"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -607,11 +620,12 @@
     <col min="2" max="2" width="16.140625" style="2" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="14" style="3" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="19" style="3" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11" style="2" bestFit="1" customWidth="1"/>
-    <col min="7" max="16384" width="9" style="2"/>
+    <col min="5" max="5" width="37.5703125" style="3" customWidth="1"/>
+    <col min="7" max="7" width="11" style="2" bestFit="1" customWidth="1"/>
+    <col min="8" max="16384" width="9" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -624,11 +638,14 @@
       <c r="D1" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="E1" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="F1" s="4" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="3">
         <v>1</v>
       </c>
@@ -641,11 +658,14 @@
       <c r="D2" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="2" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E2" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="3">
         <v>2</v>
       </c>
@@ -658,11 +678,11 @@
       <c r="D3" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="E3" s="2" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F3" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="3">
         <v>3</v>
       </c>
@@ -675,11 +695,11 @@
       <c r="D4" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="E4" s="2" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F4" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="3">
         <v>4</v>
       </c>
@@ -692,11 +712,11 @@
       <c r="D5" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="E5" s="2" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F5" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="3">
         <v>5</v>
       </c>
@@ -709,11 +729,11 @@
       <c r="D6" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="E6" s="2" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F6" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="3">
         <v>6</v>
       </c>
@@ -726,11 +746,14 @@
       <c r="D7" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="E7" s="2" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E7" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="3">
         <v>7</v>
       </c>
@@ -743,11 +766,11 @@
       <c r="D8" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="E8" s="2" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F8" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="3">
         <v>8</v>
       </c>
@@ -760,11 +783,11 @@
       <c r="D9" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="E9" s="2" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F9" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="3">
         <v>9</v>
       </c>
@@ -777,11 +800,11 @@
       <c r="D10" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="E10" s="2" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F10" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="3">
         <v>10</v>
       </c>
@@ -794,7 +817,7 @@
       <c r="D11" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="E11" s="2" t="s">
+      <c r="F11" s="2" t="s">
         <v>24</v>
       </c>
     </row>

</xml_diff>